<commit_message>
fixed bug with route
</commit_message>
<xml_diff>
--- a/util/beaconid.xlsx
+++ b/util/beaconid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaden Wong\WORK\indoor-navigation-system\backend\util\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178EE252-72B8-4993-86F4-C9899B7B9D5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166F56A6-10E9-4DA9-A211-709A89E2982F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{0DC59801-9501-4D46-ABD4-710254223A81}"/>
   </bookViews>
@@ -479,7 +479,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,10 +683,10 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <v>3.0646567450414701</v>
+        <v>3.0646523419187801</v>
       </c>
       <c r="D12">
-        <v>101.600582218984</v>
+        <v>101.600579682774</v>
       </c>
       <c r="E12">
         <v>4</v>

</xml_diff>